<commit_message>
modify mb submission excel
</commit_message>
<xml_diff>
--- a/assets/files/submission/metabobank/MetaboBank_CE-MS_metadata.xlsx
+++ b/assets/files/submission/metabobank/MetaboBank_CE-MS_metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36615" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8952"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="267">
   <si>
     <t>Study Title</t>
   </si>
@@ -781,10 +781,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Update definitions to MB-IDF-version=2022-02-18 and MB-SDRF-version=2022-02-18.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Comment[Related study]</t>
   </si>
   <si>
@@ -919,6 +915,13 @@
   <si>
     <t>Reference to Capillary Electrophoresis protocol.</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Update definitions to MB-IDF-version=2022-06-29 and MB-SDRF-version=2022-02-18.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>matrix-assisted laser desorption-ionisation mass spectrometry</t>
   </si>
 </sst>
 </file>
@@ -1434,109 +1437,109 @@
   <dimension ref="A1:B91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="126.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.875" style="4"/>
+    <col min="1" max="1" width="126.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>223</v>
       </c>
       <c r="B16" s="7">
-        <v>44645</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>44741</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>224</v>
       </c>
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>225</v>
       </c>
@@ -1544,232 +1547,232 @@
         <v>44509</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>226</v>
+        <v>265</v>
       </c>
       <c r="B20" s="7">
-        <v>44645</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>44741</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
     </row>
   </sheetData>
@@ -1788,13 +1791,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.5" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="38.44140625" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="38.5" style="10"/>
+    <col min="1" max="16384" width="38.44140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1805,19 +1808,19 @@
     </row>
     <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>196</v>
       </c>
@@ -1825,24 +1828,24 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>2</v>
       </c>
@@ -1853,7 +1856,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>3</v>
       </c>
@@ -1864,15 +1867,15 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>5</v>
       </c>
@@ -1883,7 +1886,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>6</v>
       </c>
@@ -1894,7 +1897,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>7</v>
       </c>
@@ -1905,7 +1908,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>192</v>
       </c>
@@ -1916,7 +1919,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>8</v>
       </c>
@@ -1927,15 +1930,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>10</v>
       </c>
@@ -1946,7 +1949,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>11</v>
       </c>
@@ -1957,10 +1960,10 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>12</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>52</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>53</v>
@@ -1983,7 +1986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>13</v>
       </c>
@@ -1994,7 +1997,7 @@
         <v>52</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>53</v>
@@ -2006,7 +2009,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>14</v>
       </c>
@@ -2017,7 +2020,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>15</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>130</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>131</v>
@@ -2034,7 +2037,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>16</v>
       </c>
@@ -2045,7 +2048,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>17</v>
       </c>
@@ -2056,35 +2059,35 @@
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
     </row>
-    <row r="31" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>23</v>
       </c>
@@ -2095,46 +2098,48 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="11"/>
+      <c r="B40" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>210</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>27</v>
       </c>
@@ -2168,7 +2173,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>ADMIN!$C$2:$C$26</xm:f>
+            <xm:f>ADMIN!$C$2:$C$27</xm:f>
           </x14:formula1>
           <xm:sqref>B40:G40</xm:sqref>
         </x14:dataValidation>
@@ -2189,33 +2194,33 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="48.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="48.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.625" style="10"/>
+    <col min="1" max="1" width="48.6640625" style="10"/>
     <col min="2" max="2" width="34" style="10" customWidth="1"/>
-    <col min="3" max="3" width="34.375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="27.625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="24.5" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="48.625" style="10"/>
+    <col min="3" max="3" width="34.33203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="48.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>211</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>142</v>
       </c>
@@ -2226,7 +2231,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>193</v>
       </c>
@@ -2235,7 +2240,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>194</v>
       </c>
@@ -2244,7 +2249,7 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>0</v>
       </c>
@@ -2255,7 +2260,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>1</v>
       </c>
@@ -2266,7 +2271,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>2</v>
       </c>
@@ -2277,7 +2282,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>3</v>
       </c>
@@ -2288,7 +2293,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>4</v>
       </c>
@@ -2299,10 +2304,10 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>5</v>
       </c>
@@ -2319,7 +2324,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>6</v>
       </c>
@@ -2336,12 +2341,12 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>192</v>
       </c>
@@ -2349,7 +2354,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>8</v>
       </c>
@@ -2357,21 +2362,21 @@
         <v>138</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>10</v>
       </c>
@@ -2379,7 +2384,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>11</v>
       </c>
@@ -2387,10 +2392,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="14"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>12</v>
       </c>
@@ -2398,7 +2403,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>13</v>
       </c>
@@ -2406,7 +2411,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>14</v>
       </c>
@@ -2414,7 +2419,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>15</v>
       </c>
@@ -2422,7 +2427,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>16</v>
       </c>
@@ -2430,7 +2435,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>17</v>
       </c>
@@ -2438,35 +2443,35 @@
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>24</v>
       </c>
@@ -2482,41 +2487,41 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>27</v>
       </c>
@@ -2539,58 +2544,58 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="24.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="34.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="31.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="37.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="31.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="37.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="45" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="24.875" style="3"/>
+    <col min="32" max="32" width="28.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="24.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>28</v>
       </c>
@@ -2619,7 +2624,7 @@
         <v>30</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K4" s="24" t="s">
         <v>35</v>
@@ -2691,7 +2696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
@@ -2705,7 +2710,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -2738,7 +2743,7 @@
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
@@ -2752,7 +2757,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -2785,7 +2790,7 @@
       <c r="AF6" s="11"/>
       <c r="AG6" s="11"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
@@ -2799,7 +2804,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -2832,7 +2837,7 @@
       <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="17"/>
@@ -2867,7 +2872,7 @@
       <c r="AF8" s="11"/>
       <c r="AG8" s="11"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="17"/>
@@ -2902,7 +2907,7 @@
       <c r="AF9" s="11"/>
       <c r="AG9" s="11"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="17"/>
@@ -2937,7 +2942,7 @@
       <c r="AF10" s="11"/>
       <c r="AG10" s="11"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="17"/>
@@ -2972,7 +2977,7 @@
       <c r="AF11" s="11"/>
       <c r="AG11" s="11"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="17"/>
@@ -3007,7 +3012,7 @@
       <c r="AF12" s="11"/>
       <c r="AG12" s="11"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="17"/>
@@ -3042,7 +3047,7 @@
       <c r="AF13" s="11"/>
       <c r="AG13" s="11"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="17"/>
@@ -3077,7 +3082,7 @@
       <c r="AF14" s="11"/>
       <c r="AG14" s="11"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="17"/>
@@ -3112,7 +3117,7 @@
       <c r="AF15" s="11"/>
       <c r="AG15" s="11"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="17"/>
@@ -3147,7 +3152,7 @@
       <c r="AF16" s="11"/>
       <c r="AG16" s="11"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="17"/>
@@ -3182,7 +3187,7 @@
       <c r="AF17" s="11"/>
       <c r="AG17" s="11"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="17"/>
@@ -3217,7 +3222,7 @@
       <c r="AF18" s="11"/>
       <c r="AG18" s="11"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="17"/>
@@ -3252,7 +3257,7 @@
       <c r="AF19" s="11"/>
       <c r="AG19" s="11"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="17"/>
@@ -3287,7 +3292,7 @@
       <c r="AF20" s="11"/>
       <c r="AG20" s="11"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="17"/>
@@ -3322,7 +3327,7 @@
       <c r="AF21" s="11"/>
       <c r="AG21" s="11"/>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="17"/>
@@ -3357,7 +3362,7 @@
       <c r="AF22" s="11"/>
       <c r="AG22" s="11"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="17"/>
@@ -3392,7 +3397,7 @@
       <c r="AF23" s="11"/>
       <c r="AG23" s="11"/>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="17"/>
@@ -3427,7 +3432,7 @@
       <c r="AF24" s="11"/>
       <c r="AG24" s="11"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="17"/>
@@ -3462,7 +3467,7 @@
       <c r="AF25" s="11"/>
       <c r="AG25" s="11"/>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="17"/>
@@ -3497,7 +3502,7 @@
       <c r="AF26" s="11"/>
       <c r="AG26" s="11"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="17"/>
@@ -3532,7 +3537,7 @@
       <c r="AF27" s="11"/>
       <c r="AG27" s="11"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="17"/>
@@ -3567,7 +3572,7 @@
       <c r="AF28" s="11"/>
       <c r="AG28" s="11"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="17"/>
@@ -3602,7 +3607,7 @@
       <c r="AF29" s="11"/>
       <c r="AG29" s="11"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="17"/>
@@ -3637,7 +3642,7 @@
       <c r="AF30" s="11"/>
       <c r="AG30" s="11"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="17"/>
@@ -3672,7 +3677,7 @@
       <c r="AF31" s="11"/>
       <c r="AG31" s="11"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="17"/>
@@ -3707,7 +3712,7 @@
       <c r="AF32" s="11"/>
       <c r="AG32" s="11"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="17"/>
@@ -3742,7 +3747,7 @@
       <c r="AF33" s="11"/>
       <c r="AG33" s="11"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="17"/>
@@ -3777,7 +3782,7 @@
       <c r="AF34" s="11"/>
       <c r="AG34" s="11"/>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="17"/>
@@ -3812,7 +3817,7 @@
       <c r="AF35" s="11"/>
       <c r="AG35" s="11"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="17"/>
@@ -3847,7 +3852,7 @@
       <c r="AF36" s="11"/>
       <c r="AG36" s="11"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="17"/>
@@ -3882,7 +3887,7 @@
       <c r="AF37" s="11"/>
       <c r="AG37" s="11"/>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="17"/>
@@ -3917,7 +3922,7 @@
       <c r="AF38" s="11"/>
       <c r="AG38" s="11"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="17"/>
@@ -3952,7 +3957,7 @@
       <c r="AF39" s="11"/>
       <c r="AG39" s="11"/>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="17"/>
@@ -3987,7 +3992,7 @@
       <c r="AF40" s="11"/>
       <c r="AG40" s="11"/>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="17"/>
@@ -4022,7 +4027,7 @@
       <c r="AF41" s="11"/>
       <c r="AG41" s="11"/>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="17"/>
@@ -4057,7 +4062,7 @@
       <c r="AF42" s="11"/>
       <c r="AG42" s="11"/>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="17"/>
@@ -4092,7 +4097,7 @@
       <c r="AF43" s="11"/>
       <c r="AG43" s="11"/>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="17"/>
@@ -4127,7 +4132,7 @@
       <c r="AF44" s="11"/>
       <c r="AG44" s="11"/>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="17"/>
@@ -4162,7 +4167,7 @@
       <c r="AF45" s="11"/>
       <c r="AG45" s="11"/>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="17"/>
@@ -4197,7 +4202,7 @@
       <c r="AF46" s="11"/>
       <c r="AG46" s="11"/>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="17"/>
@@ -4232,7 +4237,7 @@
       <c r="AF47" s="11"/>
       <c r="AG47" s="11"/>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="17"/>
@@ -4267,7 +4272,7 @@
       <c r="AF48" s="11"/>
       <c r="AG48" s="11"/>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="17"/>
@@ -4302,7 +4307,7 @@
       <c r="AF49" s="11"/>
       <c r="AG49" s="11"/>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="17"/>
@@ -4337,7 +4342,7 @@
       <c r="AF50" s="11"/>
       <c r="AG50" s="11"/>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
       <c r="C51" s="17"/>
@@ -4372,7 +4377,7 @@
       <c r="AF51" s="11"/>
       <c r="AG51" s="11"/>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="17"/>
@@ -4407,7 +4412,7 @@
       <c r="AF52" s="11"/>
       <c r="AG52" s="11"/>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
       <c r="C53" s="17"/>
@@ -4442,7 +4447,7 @@
       <c r="AF53" s="11"/>
       <c r="AG53" s="11"/>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="17"/>
@@ -4477,7 +4482,7 @@
       <c r="AF54" s="11"/>
       <c r="AG54" s="11"/>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="11"/>
       <c r="C55" s="17"/>
@@ -4512,7 +4517,7 @@
       <c r="AF55" s="11"/>
       <c r="AG55" s="11"/>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="B56" s="11"/>
       <c r="C56" s="17"/>
@@ -4547,7 +4552,7 @@
       <c r="AF56" s="11"/>
       <c r="AG56" s="11"/>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" s="11"/>
       <c r="C57" s="17"/>
@@ -4582,7 +4587,7 @@
       <c r="AF57" s="11"/>
       <c r="AG57" s="11"/>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
       <c r="C58" s="17"/>
@@ -4617,7 +4622,7 @@
       <c r="AF58" s="11"/>
       <c r="AG58" s="11"/>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
       <c r="C59" s="17"/>
@@ -4652,7 +4657,7 @@
       <c r="AF59" s="11"/>
       <c r="AG59" s="11"/>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="11"/>
       <c r="C60" s="17"/>
@@ -4687,7 +4692,7 @@
       <c r="AF60" s="11"/>
       <c r="AG60" s="11"/>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="11"/>
       <c r="C61" s="17"/>
@@ -4722,7 +4727,7 @@
       <c r="AF61" s="11"/>
       <c r="AG61" s="11"/>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="11"/>
       <c r="C62" s="17"/>
@@ -4757,7 +4762,7 @@
       <c r="AF62" s="11"/>
       <c r="AG62" s="11"/>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
       <c r="C63" s="17"/>
@@ -4792,7 +4797,7 @@
       <c r="AF63" s="11"/>
       <c r="AG63" s="11"/>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
       <c r="C64" s="17"/>
@@ -4827,7 +4832,7 @@
       <c r="AF64" s="11"/>
       <c r="AG64" s="11"/>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="11"/>
       <c r="C65" s="17"/>
@@ -4862,7 +4867,7 @@
       <c r="AF65" s="11"/>
       <c r="AG65" s="11"/>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="11"/>
       <c r="C66" s="18"/>
@@ -4897,7 +4902,7 @@
       <c r="AF66" s="11"/>
       <c r="AG66" s="11"/>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
       <c r="C67" s="18"/>
@@ -4932,7 +4937,7 @@
       <c r="AF67" s="11"/>
       <c r="AG67" s="11"/>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
       <c r="C68" s="18"/>
@@ -4967,7 +4972,7 @@
       <c r="AF68" s="11"/>
       <c r="AG68" s="11"/>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="11"/>
       <c r="C69" s="18"/>
@@ -5002,7 +5007,7 @@
       <c r="AF69" s="11"/>
       <c r="AG69" s="11"/>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="11"/>
       <c r="C70" s="18"/>
@@ -5037,7 +5042,7 @@
       <c r="AF70" s="11"/>
       <c r="AG70" s="11"/>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
       <c r="C71" s="18"/>
@@ -5072,7 +5077,7 @@
       <c r="AF71" s="11"/>
       <c r="AG71" s="11"/>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="11"/>
       <c r="C72" s="18"/>
@@ -5107,7 +5112,7 @@
       <c r="AF72" s="11"/>
       <c r="AG72" s="11"/>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="11"/>
       <c r="C73" s="18"/>
@@ -5142,7 +5147,7 @@
       <c r="AF73" s="11"/>
       <c r="AG73" s="11"/>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="11"/>
       <c r="C74" s="18"/>
@@ -5177,7 +5182,7 @@
       <c r="AF74" s="11"/>
       <c r="AG74" s="11"/>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="11"/>
       <c r="C75" s="18"/>
@@ -5212,7 +5217,7 @@
       <c r="AF75" s="11"/>
       <c r="AG75" s="11"/>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="11"/>
       <c r="C76" s="18"/>
@@ -5247,7 +5252,7 @@
       <c r="AF76" s="11"/>
       <c r="AG76" s="11"/>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
       <c r="C77" s="18"/>
@@ -5282,7 +5287,7 @@
       <c r="AF77" s="11"/>
       <c r="AG77" s="11"/>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
       <c r="C78" s="18"/>
@@ -5317,7 +5322,7 @@
       <c r="AF78" s="11"/>
       <c r="AG78" s="11"/>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
       <c r="C79" s="18"/>
@@ -5352,7 +5357,7 @@
       <c r="AF79" s="11"/>
       <c r="AG79" s="11"/>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="11"/>
       <c r="C80" s="18"/>
@@ -5387,7 +5392,7 @@
       <c r="AF80" s="11"/>
       <c r="AG80" s="11"/>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="11"/>
       <c r="C81" s="18"/>
@@ -5422,7 +5427,7 @@
       <c r="AF81" s="11"/>
       <c r="AG81" s="11"/>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
       <c r="C82" s="18"/>
@@ -5457,7 +5462,7 @@
       <c r="AF82" s="11"/>
       <c r="AG82" s="11"/>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
       <c r="C83" s="18"/>
@@ -5492,7 +5497,7 @@
       <c r="AF83" s="11"/>
       <c r="AG83" s="11"/>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="11"/>
       <c r="C84" s="18"/>
@@ -5527,7 +5532,7 @@
       <c r="AF84" s="11"/>
       <c r="AG84" s="11"/>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="11"/>
       <c r="C85" s="18"/>
@@ -5562,7 +5567,7 @@
       <c r="AF85" s="11"/>
       <c r="AG85" s="11"/>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
       <c r="C86" s="18"/>
@@ -5597,7 +5602,7 @@
       <c r="AF86" s="11"/>
       <c r="AG86" s="11"/>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
       <c r="B87" s="11"/>
       <c r="C87" s="18"/>
@@ -5632,7 +5637,7 @@
       <c r="AF87" s="11"/>
       <c r="AG87" s="11"/>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
       <c r="C88" s="18"/>
@@ -5667,7 +5672,7 @@
       <c r="AF88" s="11"/>
       <c r="AG88" s="11"/>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89" s="11"/>
       <c r="B89" s="11"/>
       <c r="C89" s="18"/>
@@ -5702,7 +5707,7 @@
       <c r="AF89" s="11"/>
       <c r="AG89" s="11"/>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
       <c r="B90" s="11"/>
       <c r="C90" s="18"/>
@@ -5737,7 +5742,7 @@
       <c r="AF90" s="11"/>
       <c r="AG90" s="11"/>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91" s="11"/>
       <c r="B91" s="11"/>
       <c r="C91" s="18"/>
@@ -5772,7 +5777,7 @@
       <c r="AF91" s="11"/>
       <c r="AG91" s="11"/>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
       <c r="B92" s="11"/>
       <c r="C92" s="18"/>
@@ -5807,7 +5812,7 @@
       <c r="AF92" s="11"/>
       <c r="AG92" s="11"/>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
       <c r="B93" s="11"/>
       <c r="C93" s="18"/>
@@ -5842,7 +5847,7 @@
       <c r="AF93" s="11"/>
       <c r="AG93" s="11"/>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
       <c r="B94" s="11"/>
       <c r="C94" s="18"/>
@@ -5877,7 +5882,7 @@
       <c r="AF94" s="11"/>
       <c r="AG94" s="11"/>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95" s="11"/>
       <c r="B95" s="11"/>
       <c r="C95" s="18"/>
@@ -5912,7 +5917,7 @@
       <c r="AF95" s="11"/>
       <c r="AG95" s="11"/>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96" s="11"/>
       <c r="B96" s="11"/>
       <c r="C96" s="18"/>
@@ -5947,7 +5952,7 @@
       <c r="AF96" s="11"/>
       <c r="AG96" s="11"/>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A97" s="11"/>
       <c r="B97" s="11"/>
       <c r="C97" s="18"/>
@@ -5982,7 +5987,7 @@
       <c r="AF97" s="11"/>
       <c r="AG97" s="11"/>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A98" s="11"/>
       <c r="B98" s="11"/>
       <c r="C98" s="18"/>
@@ -6017,7 +6022,7 @@
       <c r="AF98" s="11"/>
       <c r="AG98" s="11"/>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A99" s="11"/>
       <c r="B99" s="11"/>
       <c r="C99" s="18"/>
@@ -6052,7 +6057,7 @@
       <c r="AF99" s="11"/>
       <c r="AG99" s="11"/>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A100" s="11"/>
       <c r="B100" s="11"/>
       <c r="C100" s="18"/>
@@ -6087,7 +6092,7 @@
       <c r="AF100" s="11"/>
       <c r="AG100" s="11"/>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A101" s="11"/>
       <c r="B101" s="11"/>
       <c r="C101" s="18"/>
@@ -6122,7 +6127,7 @@
       <c r="AF101" s="11"/>
       <c r="AG101" s="11"/>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A102" s="11"/>
       <c r="B102" s="11"/>
       <c r="C102" s="18"/>
@@ -6157,7 +6162,7 @@
       <c r="AF102" s="11"/>
       <c r="AG102" s="11"/>
     </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A103" s="11"/>
       <c r="B103" s="11"/>
       <c r="C103" s="18"/>
@@ -6192,7 +6197,7 @@
       <c r="AF103" s="11"/>
       <c r="AG103" s="11"/>
     </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A104" s="11"/>
       <c r="B104" s="11"/>
       <c r="C104" s="18"/>
@@ -6227,7 +6232,7 @@
       <c r="AF104" s="11"/>
       <c r="AG104" s="11"/>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>
       <c r="B105" s="11"/>
       <c r="C105" s="18"/>
@@ -6282,30 +6287,30 @@
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="37.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.875" style="10"/>
-    <col min="3" max="4" width="37.875" style="28"/>
-    <col min="5" max="16384" width="37.875" style="10"/>
+    <col min="1" max="1" width="48.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" style="10"/>
+    <col min="3" max="4" width="37.88671875" style="28"/>
+    <col min="5" max="16384" width="37.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>165</v>
@@ -6315,7 +6320,7 @@
       </c>
       <c r="D4" s="30"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>28</v>
       </c>
@@ -6327,7 +6332,7 @@
       </c>
       <c r="D5" s="30"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>29</v>
       </c>
@@ -6337,7 +6342,7 @@
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>30</v>
       </c>
@@ -6347,7 +6352,7 @@
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>31</v>
       </c>
@@ -6357,7 +6362,7 @@
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>30</v>
       </c>
@@ -6367,9 +6372,9 @@
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>171</v>
@@ -6377,7 +6382,7 @@
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>33</v>
       </c>
@@ -6387,9 +6392,9 @@
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>173</v>
@@ -6397,37 +6402,37 @@
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>259</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>36</v>
       </c>
@@ -6437,17 +6442,17 @@
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>38</v>
       </c>
@@ -6457,7 +6462,7 @@
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>39</v>
       </c>
@@ -6467,7 +6472,7 @@
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>30</v>
       </c>
@@ -6477,7 +6482,7 @@
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>40</v>
       </c>
@@ -6487,7 +6492,7 @@
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>41</v>
       </c>
@@ -6497,7 +6502,7 @@
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>42</v>
       </c>
@@ -6507,7 +6512,7 @@
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>43</v>
       </c>
@@ -6517,7 +6522,7 @@
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>44</v>
       </c>
@@ -6527,7 +6532,7 @@
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>45</v>
       </c>
@@ -6537,7 +6542,7 @@
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>46</v>
       </c>
@@ -6547,7 +6552,7 @@
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>47</v>
       </c>
@@ -6557,7 +6562,7 @@
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>202</v>
       </c>
@@ -6567,7 +6572,7 @@
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>30</v>
       </c>
@@ -6577,7 +6582,7 @@
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>48</v>
       </c>
@@ -6587,7 +6592,7 @@
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>203</v>
       </c>
@@ -6597,7 +6602,7 @@
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>30</v>
       </c>
@@ -6607,7 +6612,7 @@
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>208</v>
       </c>
@@ -6617,7 +6622,7 @@
       <c r="C34" s="30"/>
       <c r="D34" s="30"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>200</v>
       </c>
@@ -6627,7 +6632,7 @@
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>204</v>
       </c>
@@ -6637,7 +6642,7 @@
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>50</v>
       </c>
@@ -6647,107 +6652,107 @@
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C38" s="30"/>
       <c r="D38" s="30"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C40" s="30"/>
       <c r="D40" s="30"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C41" s="30"/>
       <c r="D41" s="30"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C42" s="30"/>
       <c r="D42" s="30"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C43" s="30"/>
       <c r="D43" s="30"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C44" s="30"/>
       <c r="D44" s="30"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C46" s="30"/>
       <c r="D46" s="30"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="30"/>
       <c r="D50" s="30"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" s="30"/>
       <c r="D52" s="30"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="30"/>
       <c r="D54" s="30"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="30"/>
       <c r="D56" s="30"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="30"/>
       <c r="D57" s="30"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="30"/>
       <c r="D58" s="30"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" s="30"/>
       <c r="D60" s="30"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" s="30"/>
       <c r="D61" s="30"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C62" s="30"/>
       <c r="D62" s="30"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C63" s="30"/>
       <c r="D63" s="30"/>
     </row>
@@ -6763,18 +6768,18 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C2" sqref="C2:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.875" style="3"/>
+    <col min="3" max="3" width="96.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>56</v>
       </c>
@@ -6785,7 +6790,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -6796,7 +6801,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
@@ -6804,10 +6809,10 @@
         <v>62</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>83</v>
       </c>
@@ -6815,12 +6820,12 @@
         <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>66</v>
@@ -6829,9 +6834,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>68</v>
@@ -6840,9 +6845,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>70</v>
@@ -6851,9 +6856,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>72</v>
@@ -6862,9 +6867,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>74</v>
@@ -6873,7 +6878,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>61</v>
       </c>
@@ -6884,7 +6889,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>63</v>
       </c>
@@ -6895,18 +6900,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>67</v>
       </c>
@@ -6914,10 +6919,10 @@
         <v>82</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>69</v>
       </c>
@@ -6928,7 +6933,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>71</v>
       </c>
@@ -6936,10 +6941,10 @@
         <v>89</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>73</v>
       </c>
@@ -6950,7 +6955,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>75</v>
       </c>
@@ -6958,10 +6963,10 @@
         <v>119</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
@@ -6969,10 +6974,10 @@
         <v>93</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>79</v>
       </c>
@@ -6980,10 +6985,10 @@
         <v>95</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>81</v>
       </c>
@@ -6991,10 +6996,10 @@
         <v>97</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>85</v>
       </c>
@@ -7002,10 +7007,10 @@
         <v>121</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>88</v>
       </c>
@@ -7013,103 +7018,106 @@
         <v>98</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Labeled Extract Name made optional
</commit_message>
<xml_diff>
--- a/assets/files/submission/metabobank/MetaboBank_CE-MS_metadata.xlsx
+++ b/assets/files/submission/metabobank/MetaboBank_CE-MS_metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8952"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="269">
   <si>
     <t>Study Title</t>
   </si>
@@ -588,14 +588,6 @@
     <t>Manufacturer, model number and dimensions.</t>
   </si>
   <si>
-    <t>A unique identifier from a particular labeled extract. Use a sample name of BioSample in most cases.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>If you used a chemical or biochemical marker in the sample such as a radioactive isotope of fluorescent dye which is bound to a material in order to make it detectable in an analytical instrument then enter it here.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Reference to Mass spectrometry protocol.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -922,6 +914,20 @@
   </si>
   <si>
     <t>matrix-assisted laser desorption-ionisation mass spectrometry</t>
+  </si>
+  <si>
+    <t>Labeled Extract Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Labeled Extract Name was made optional.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>When samples are chemically labeled by isotopes (chemical isotope labeling), describe isotopes in the Label column and isotope-labeled compounds in the Comment[isotope_labeled_compound] column.</t>
+  </si>
+  <si>
+    <t>A unique identifier from a particular extract chemically labeled by isotopes. Optional for non-labeled samples.</t>
   </si>
 </sst>
 </file>
@@ -1436,9 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1449,52 +1453,52 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1503,19 +1507,19 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1523,7 +1527,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B16" s="7">
         <v>44741</v>
@@ -1535,13 +1539,13 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B19" s="7">
         <v>44509</v>
@@ -1549,15 +1553,19 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B20" s="7">
         <v>44741</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B21" s="7">
+        <v>44802</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1791,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -1802,13 +1810,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B2" s="9"/>
     </row>
@@ -1822,7 +1830,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B5" s="10">
         <v>1.1000000000000001</v>
@@ -1830,7 +1838,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1910,7 +1918,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1935,7 +1943,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1974,7 +1982,7 @@
         <v>52</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>53</v>
@@ -1997,7 +2005,7 @@
         <v>52</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>53</v>
@@ -2029,7 +2037,7 @@
         <v>130</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>131</v>
@@ -2113,10 +2121,10 @@
     </row>
     <row r="41" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2126,12 +2134,12 @@
     </row>
     <row r="43" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2206,13 +2214,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B2" s="9"/>
     </row>
@@ -2233,19 +2241,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -2348,7 +2356,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>137</v>
@@ -2362,13 +2370,13 @@
         <v>138</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2489,7 +2497,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2497,23 +2505,23 @@
         <v>25</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2540,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG105"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2584,12 +2592,12 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -2624,7 +2632,7 @@
         <v>30</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K4" s="24" t="s">
         <v>35</v>
@@ -2635,8 +2643,8 @@
       <c r="M4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="21" t="s">
-        <v>38</v>
+      <c r="N4" s="24" t="s">
+        <v>265</v>
       </c>
       <c r="O4" s="24" t="s">
         <v>39</v>
@@ -2669,7 +2677,7 @@
         <v>47</v>
       </c>
       <c r="Y4" s="21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Z4" s="21" t="s">
         <v>30</v>
@@ -2678,7 +2686,7 @@
         <v>48</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AC4" s="21" t="s">
         <v>30</v>
@@ -2687,10 +2695,10 @@
         <v>49</v>
       </c>
       <c r="AE4" s="21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AF4" s="21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AG4" s="21" t="s">
         <v>50</v>
@@ -2710,7 +2718,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -2757,7 +2765,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -2804,7 +2812,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -6284,7 +6292,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6297,12 +6305,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6310,7 +6318,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>165</v>
@@ -6328,7 +6336,7 @@
         <v>168</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D5" s="30"/>
     </row>
@@ -6374,7 +6382,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>171</v>
@@ -6394,7 +6402,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>173</v>
@@ -6407,17 +6415,17 @@
         <v>30</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
@@ -6427,7 +6435,7 @@
         <v>35</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -6447,17 +6455,17 @@
         <v>37</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>175</v>
+        <v>268</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -6467,7 +6475,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>176</v>
+        <v>267</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
@@ -6477,7 +6485,7 @@
         <v>30</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
@@ -6487,7 +6495,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -6497,7 +6505,7 @@
         <v>41</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -6507,7 +6515,7 @@
         <v>42</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -6517,7 +6525,7 @@
         <v>43</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
@@ -6527,7 +6535,7 @@
         <v>44</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -6537,7 +6545,7 @@
         <v>45</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
@@ -6547,7 +6555,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -6557,17 +6565,17 @@
         <v>47</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -6577,7 +6585,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>
@@ -6587,17 +6595,17 @@
         <v>48</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
@@ -6607,37 +6615,37 @@
         <v>30</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
@@ -6647,7 +6655,7 @@
         <v>50</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
@@ -6809,7 +6817,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6820,12 +6828,12 @@
         <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>66</v>
@@ -6836,7 +6844,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>68</v>
@@ -6847,7 +6855,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>70</v>
@@ -6858,7 +6866,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>72</v>
@@ -6869,7 +6877,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>74</v>
@@ -6905,7 +6913,7 @@
         <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>103</v>
@@ -6919,7 +6927,7 @@
         <v>82</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6941,7 +6949,7 @@
         <v>89</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -7018,12 +7026,12 @@
         <v>98</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>123</v>
@@ -7034,7 +7042,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>125</v>
@@ -7064,7 +7072,7 @@
         <v>104</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MB fields explanation added, excel HELP tabs deleted
</commit_message>
<xml_diff>
--- a/assets/files/submission/metabobank/MetaboBank_CE-MS_metadata.xlsx
+++ b/assets/files/submission/metabobank/MetaboBank_CE-MS_metadata.xlsx
@@ -4,18 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17436" windowHeight="11124"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="12" r:id="rId1"/>
     <sheet name="MB_Study_IDF" sheetId="2" r:id="rId2"/>
-    <sheet name="MB_Study_IDF HELP" sheetId="14" r:id="rId3"/>
-    <sheet name="MB_Assay_SDRF" sheetId="3" r:id="rId4"/>
-    <sheet name="MB_Assay_SDRF HELP" sheetId="15" r:id="rId5"/>
-    <sheet name="ADMIN" sheetId="10" r:id="rId6"/>
+    <sheet name="MB_Assay_SDRF" sheetId="3" r:id="rId3"/>
+    <sheet name="ADMIN" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ADMIN!$A$1:$C$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ADMIN!$A$1:$C$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="184">
   <si>
     <t>Study Title</t>
   </si>
@@ -143,9 +141,6 @@
     <t>Parameter Value[Column type]</t>
   </si>
   <si>
-    <t>Labeled Extract Name</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -423,251 +418,24 @@
   </si>
   <si>
     <t>Scan polarity;Scan m/z range;Instrument;Ion source;Mass analyzer</t>
-  </si>
-  <si>
-    <t>The overall title of the study. This field can only have one value.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A short paragraph describing the study as free-text. This tag can only have one value. The text should clearly explain what you did in your experiment - this will help the curation team to check and process your submission.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A term describing the type of each experimental factor.</t>
-  </si>
-  <si>
-    <t>The experiment design types which are applicable to this study. These terms should come from controlled terms.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A user-defined name for each experimental factor studied by the experiment. These experimental factors represent the variables within the investigation (e.g. growth condition, genotype, organism part). The actual values of these variables will be listed in the SDRF file, in "Ffactor value[&lt;factor name&gt;]" columns.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The organization affiliation for each person associated with the study.</t>
-  </si>
-  <si>
-    <t>The role(s) performed by each person. Only “submitter” role is permitted.</t>
-  </si>
-  <si>
-    <t>The last name of each submitter. Enter last names of submitters in each column.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The first name of each submitter. Enter first names of submitters in each column.</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t># Fields without line boxes can have multiple values in corresponding columns.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Field</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Readme</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Example</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Correlation-based Deconvolution (CorrDec) to generate high quality MS2 spectra from data independent acquisition in multi-sample studies (Chemical standards assay)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Data-independent acquisition mass spectrometry (DIA-MS) is essential for information-rich spectral annotations in untargeted metabolomics. However, the acquired MS2 spectra are highly complex, posing significant annotation challenges. We have developed a correlation-based deconvolution (CorrDec) method that uses ion abundance correlations in multi-sample studies using DIA-MS as an update of our MS-DIAL software. CorrDec is based on the assumption that peak intensities of precursor and fragment ions correlate across samples, and exploits this quantitative information to deconvolute complex DIA spectra. CorrDec clearly improved deconvolution of the original MS-DIAL deconvolution method (MS2Dec) in a dilution series of chemical standards and a 224-sample urinary metabolomics study. The primary advantage of CorrDec over MS2Dec is the ability to discriminate co-eluting low-abundance compounds. CorrDec requires the measurement of multiple samples to successfully deconvolute DIA spectra, and our randomized assessment demonstrated that CorrDec can contribute to studies with as few as 10 unique samples. The presented methodology improves compound annotation and identification in multi-sample studies and will be useful for applications in large cohort studies.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dose response design</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>concentration</t>
-  </si>
-  <si>
-    <t>Mishima</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Tarou</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Fuji</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Saburo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Rakuju</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Sonoko</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The PubMed IDs of the publication(s) associated with this study (where available).</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A Digital Object Identifier (DOI) for each publication (where available). When PubMed ID and DOI are available, use PubMed ID.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The names of the protocols used.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A free-text description of the protocol. This text is included in a single tab-delimited field.</t>
-  </si>
-  <si>
-    <t>A semicolon-delimited list of parameter names.</t>
-  </si>
-  <si>
-    <t>The protocol hardware is the instrument that was use to capture the sample. If multiple instruments are used, they should be separated by (;)</t>
-  </si>
-  <si>
-    <t>The software used by the protocol.</t>
-  </si>
-  <si>
-    <t>The type of the protocol.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The study types which are applicable to this study. These terms should come from controlled terms.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The experiment types which are applicable to this study. These terms should come from controlled terms.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Readme</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Sample attributes. Use BioSample attributes.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Reference to Sample collection protocol.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A unique identifier from a particular source. Use a sample name of BioSample in most cases.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A unique identifier from a particular sample. Use a sample name of BioSample in most cases.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Reference to Extraction protocol.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>This column describes how the sample was extracted into a solvent prior to being injected into the analytical instrument of choice.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>If the sample has been subjected to chemical modification prior to injection.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A unique identifier from a particular extract. Use a sample name of BioSample in most cases.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Manufacturer, model number and dimensions.</t>
-  </si>
-  <si>
-    <t>Reference to Mass spectrometry protocol.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The range used in the assay.</t>
-  </si>
-  <si>
-    <t>Ion source of the instrument where applicable.</t>
-  </si>
-  <si>
-    <t>The analyser/detector of the mass fragments generated during the assay.</t>
-  </si>
-  <si>
-    <t>‘positive’, ‘negative’ or 'alternating'</t>
-  </si>
-  <si>
-    <t>Add the full name of the instrument you used for the MS study in this assay, including the model number.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A unique identifier from a particular assay name. Use a sample name of BioSample in most cases. Technical replicates are differentiated by same sample names, different assay names and technical replicate comments.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Technical replicates such as 1, 2 and 3.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>This is where you should enter the raw (unprocessed) MS data files. Please add the filename in the cell.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Data processing</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>If your data has been processed into one of the open-source raw data formats e.g. mzML, nmrML, then add them here.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Metabolite identification</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A TSV file containing information about the metabolites investigated in the study. Information regarding database accession IDs , where in the spectra the metabolite is found and data pertaining to its abundance within the study samples should be in this file.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>The factor values for an experiment are the values of the variables under investigation. For example, an experiment studying the effect of different temparature (heat stress) on a cell culture would have “temparature” as an experimental variable with “Unit” column to indicate the unit.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>decorative_physalis_leaves</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Person Email</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Comment[MetaboBank accession]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>MAGE-TAB Version</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Comment[MetaboBank accession]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Version number of MAGE-TAB.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MAGE-TAB Version</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Accession number issed by Metabobank</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Comment[Processed Data File md5]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -684,38 +452,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Comment[Raw Data File md5]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Comment[Processed Data File md5]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Comment[maf_value_unit]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Enter md5 hash value of Raw Data File here.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MD5 hash value of Processed Data File here.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Enter MD5 hash value of Comment[Metabolite Assignment File here.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Metabolite Assignment File</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Value unit usiing for the experimental data in Metabolite Assignment File. (e.g. "peak area", "pico mole" etc.)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Comment[Submission type]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -724,10 +460,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t># Study (IDF) fields</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t># Assay (SDRF) columns</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -773,28 +505,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Comment[Related study]</t>
-  </si>
-  <si>
-    <t>Comment[Contributor]</t>
-  </si>
-  <si>
-    <t>Bioinformation and DDBJ Center</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Field</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Extract Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Parameter Value[Post extraction]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>metabolite target analysis</t>
   </si>
   <si>
@@ -838,10 +548,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t># See HELP tabs to view definition, or see https://www.ddbj.nig.ac.jp/metabobank</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Uneditable</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -854,24 +560,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Related study database ID.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>BioProject ID.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Name of each contributer.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Manufacturer and model number.</t>
-  </si>
-  <si>
-    <t>Type or phase of column used.</t>
-  </si>
-  <si>
     <t>CE-MS</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -883,9 +571,6 @@
     <t>Parameter Value[CE instrument]</t>
   </si>
   <si>
-    <t>Add the full name of the instrument you used for the CE part of this assay, including the manufacturer and model number as reported in manufacturer’s brochures, user manuals, or on their website.</t>
-  </si>
-  <si>
     <t># Submission type: MS Capillary electrophoresis - CE (CE-MS)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -905,10 +590,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Reference to Capillary Electrophoresis protocol.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Update definitions to MB-IDF-version=2022-06-29 and MB-SDRF-version=2022-02-18.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -924,10 +605,8 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>When samples are chemically labeled by isotopes (chemical isotope labeling), describe isotopes in the Label column and isotope-labeled compounds in the Comment[isotope_labeled_compound] column.</t>
-  </si>
-  <si>
-    <t>A unique identifier from a particular extract chemically labeled by isotopes. Optional for non-labeled samples.</t>
+    <t># To view definition, see https://www.ddbj.nig.ac.jp/metabobank/metadata-e.html</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1057,7 +736,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1088,28 +767,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1453,52 +1114,52 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>258</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>244</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>215</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>217</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>218</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,19 +1168,19 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4" t="s">
-        <v>219</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>220</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
-        <v>245</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1527,10 +1188,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
       <c r="B16" s="7">
-        <v>44741</v>
+        <v>44848</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1539,13 +1200,13 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>223</v>
+        <v>153</v>
       </c>
       <c r="B19" s="7">
         <v>44509</v>
@@ -1553,7 +1214,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>263</v>
+        <v>179</v>
       </c>
       <c r="B20" s="7">
         <v>44741</v>
@@ -1561,7 +1222,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>266</v>
+        <v>182</v>
       </c>
       <c r="B21" s="7">
         <v>44802</v>
@@ -1810,13 +1471,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>259</v>
+        <v>176</v>
       </c>
       <c r="B2" s="9"/>
     </row>
@@ -1825,12 +1486,12 @@
     </row>
     <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>194</v>
+        <v>134</v>
       </c>
       <c r="B5" s="10">
         <v>1.1000000000000001</v>
@@ -1838,7 +1499,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>192</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1918,7 +1579,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1943,11 +1604,11 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>243</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="11"/>
@@ -1958,7 +1619,7 @@
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="11"/>
@@ -1972,26 +1633,26 @@
       <c r="B23" s="12"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="D24" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1999,22 +1660,22 @@
         <v>13</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="E25" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2029,24 +1690,24 @@
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="11"/>
@@ -2057,7 +1718,7 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="11"/>
@@ -2111,7 +1772,7 @@
         <v>24</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -2121,25 +1782,25 @@
     </row>
     <row r="41" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>208</v>
+        <v>139</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>253</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
-        <v>247</v>
+      <c r="A43" s="24" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
-        <v>246</v>
+      <c r="A44" s="24" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2195,356 +1856,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="48.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.6640625" style="10"/>
-    <col min="2" max="2" width="34" style="10" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="48.6640625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B2" s="9"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="5" max="1048575" man="1"/>
-  </colBreaks>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG105"/>
   <sheetViews>
@@ -2592,12 +1903,12 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>211</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>259</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -2619,10 +1930,10 @@
       <c r="E4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="21" t="s">
@@ -2631,94 +1942,94 @@
       <c r="I4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="K4" s="24" t="s">
+      <c r="J4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="K4" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>39</v>
+      <c r="N4" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="P4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="S4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="T4" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="T4" s="24" t="s">
+      <c r="U4" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="V4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="W4" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="24" t="s">
+      <c r="X4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="X4" s="21" t="s">
-        <v>47</v>
-      </c>
       <c r="Y4" s="21" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="Z4" s="21" t="s">
         <v>30</v>
       </c>
       <c r="AA4" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
       <c r="AC4" s="21" t="s">
         <v>30</v>
       </c>
       <c r="AD4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG4" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="AE4" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF4" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="AG4" s="21" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>261</v>
+        <v>178</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -2727,7 +2038,7 @@
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
@@ -2739,12 +2050,12 @@
       <c r="X5" s="11"/>
       <c r="Y5" s="11"/>
       <c r="Z5" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
@@ -2755,17 +2066,17 @@
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>260</v>
+        <v>177</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -2774,7 +2085,7 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
@@ -2786,12 +2097,12 @@
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
       <c r="Z6" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA6" s="11"/>
       <c r="AB6" s="11"/>
       <c r="AC6" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
@@ -2802,17 +2113,17 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>260</v>
+        <v>177</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -2821,7 +2132,7 @@
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
@@ -2833,12 +2144,12 @@
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
@@ -6287,491 +5598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="37.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" style="10"/>
-    <col min="3" max="4" width="37.88671875" style="28"/>
-    <col min="5" max="16384" width="37.88671875" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="30"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="30"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>255</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
@@ -6789,345 +5616,345 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>238</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>239</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>231</v>
+        <v>155</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>232</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>233</v>
+        <v>157</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>234</v>
+        <v>158</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>237</v>
+        <v>161</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>240</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>264</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>241</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>235</v>
+        <v>159</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>236</v>
+        <v>160</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>242</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>